<commit_message>
Options GUI, more validation, tests
</commit_message>
<xml_diff>
--- a/src/test/resources/ListaSvincolatiShort3.xlsx
+++ b/src/test/resources/ListaSvincolatiShort3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="40" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="12080" yWindow="340" windowWidth="25360" windowHeight="15820"/>
   </bookViews>
   <sheets>
     <sheet name="ListaSvincolati" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -614,9 +614,6 @@
       </c>
       <c r="D12">
         <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:5">

</xml_diff>